<commit_message>
sửa demo excel doanh nghiệp
</commit_message>
<xml_diff>
--- a/storage/app/private/test_doanh_nghiep.xlsx
+++ b/storage/app/private/test_doanh_nghiep.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Tên doanh nghiệp</t>
   </si>
@@ -48,20 +48,72 @@
     <t>Công nghệ khác</t>
   </si>
   <si>
-    <t>this is test</t>
+    <t>test1@gmail.com</t>
+  </si>
+  <si>
+    <t>test2@gmail.com</t>
+  </si>
+  <si>
+    <t>test4@gmail.com</t>
+  </si>
+  <si>
+    <t>test3@gmail.com</t>
+  </si>
+  <si>
+    <t>test5@gmail.com</t>
+  </si>
+  <si>
+    <t>test6@gmail.com</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn A</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn B</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn C</t>
+  </si>
+  <si>
+    <t>Doanh nghiệp A</t>
+  </si>
+  <si>
+    <t>Doanh nghiệp B</t>
+  </si>
+  <si>
+    <t>Doanh nghiệp C</t>
+  </si>
+  <si>
+    <t>144 Xuân Thủy, Cầu Giấy, Hà Nội</t>
+  </si>
+  <si>
+    <t>145 Xuân Thủy, Cầu Giấy, Hà Nội</t>
+  </si>
+  <si>
+    <t>146 Xuân Thủy, Cầu Giấy, Hà Nội</t>
+  </si>
+  <si>
+    <t>25 Lê Thánh Tông, Hoàn Kiếm, Hà Nội</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,19 +133,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -389,17 +444,17 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
@@ -420,7 +475,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -432,22 +487,22 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -458,22 +513,22 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -484,10 +539,22 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -497,7 +564,16 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="E3" r:id="rId5"/>
+    <hyperlink ref="E4" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 

</xml_diff>